<commit_message>
excel frame mit for schleife
</commit_message>
<xml_diff>
--- a/Hannes/output.xlsx
+++ b/Hannes/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C3:E4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,26 +433,40 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3">
-      <c r="C3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hue</t>
+        </is>
       </c>
     </row>
-    <row r="4">
-      <c r="C4" t="n">
-        <v>80.70174708472403</v>
-      </c>
-      <c r="D4" t="n">
-        <v>109.4445702204873</v>
-      </c>
-      <c r="E4" t="n">
-        <v>130.718626969528</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>86.87834324477781</v>
+      </c>
+      <c r="B2" t="n">
+        <v>118.4321638824971</v>
+      </c>
+      <c r="C2" t="n">
+        <v>148.4725517736007</v>
+      </c>
+      <c r="D2" t="n">
+        <v>86.87834324477781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alle features in einer funktion
</commit_message>
<xml_diff>
--- a/Hannes/output.xlsx
+++ b/Hannes/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,105 +439,495 @@
           <t>contour number</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>aspect ratio</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>extent</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Hue</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>28</v>
+        <v>65</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1719789131198317</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.8982768326077035</v>
+      </c>
+      <c r="D2" t="n">
+        <v>29.20517301642782</v>
+      </c>
+      <c r="E2" t="n">
+        <v>87.63998601887452</v>
+      </c>
+      <c r="F2" t="n">
+        <v>111.1006641034603</v>
+      </c>
+      <c r="G2" t="n">
+        <v>15.91261796574624</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.1827491780715877</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.8435412556136059</v>
+      </c>
+      <c r="D3" t="n">
+        <v>34.04604726976365</v>
+      </c>
+      <c r="E3" t="n">
+        <v>89.2322738386308</v>
+      </c>
+      <c r="F3" t="n">
+        <v>113.4099429502852</v>
+      </c>
+      <c r="G3" t="n">
+        <v>14.28198859005705</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.2001229539807216</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8239227184043145</v>
+      </c>
+      <c r="D4" t="n">
+        <v>36.64510412051396</v>
+      </c>
+      <c r="E4" t="n">
+        <v>89.1856446610545</v>
+      </c>
+      <c r="F4" t="n">
+        <v>111.1789986708019</v>
+      </c>
+      <c r="G4" t="n">
+        <v>18.83473637571998</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>31</v>
+        <v>57</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1724024047621364</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8603092840105619</v>
+      </c>
+      <c r="D5" t="n">
+        <v>29.96866230121609</v>
+      </c>
+      <c r="E5" t="n">
+        <v>83.80308699719365</v>
+      </c>
+      <c r="F5" t="n">
+        <v>106.6721234798877</v>
+      </c>
+      <c r="G5" t="n">
+        <v>18.93592142188962</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1709531994201213</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.8511780904461099</v>
+      </c>
+      <c r="D6" t="n">
+        <v>28.61282771535581</v>
+      </c>
+      <c r="E6" t="n">
+        <v>88.08192883895131</v>
+      </c>
+      <c r="F6" t="n">
+        <v>106.3909176029963</v>
+      </c>
+      <c r="G6" t="n">
+        <v>16.80571161048689</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1705332642443037</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8710008561078881</v>
+      </c>
+      <c r="D7" t="n">
+        <v>34.12296650717703</v>
+      </c>
+      <c r="E7" t="n">
+        <v>90.38612440191388</v>
+      </c>
+      <c r="F7" t="n">
+        <v>111.6253588516746</v>
+      </c>
+      <c r="G7" t="n">
+        <v>15.99760765550239</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1765076877759789</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8434846771593958</v>
+      </c>
+      <c r="D8" t="n">
+        <v>28.2516156828953</v>
+      </c>
+      <c r="E8" t="n">
+        <v>89.32701421800948</v>
+      </c>
+      <c r="F8" t="n">
+        <v>112.2856527358897</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.57690650581646</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>39</v>
+        <v>61</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1645684068006661</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8994874721960268</v>
+      </c>
+      <c r="D9" t="n">
+        <v>28.53610988037218</v>
+      </c>
+      <c r="E9" t="n">
+        <v>82.89455028799291</v>
+      </c>
+      <c r="F9" t="n">
+        <v>108.7771377935312</v>
+      </c>
+      <c r="G9" t="n">
+        <v>16.07665042091272</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.1660514160824168</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8758838208671624</v>
+      </c>
+      <c r="D10" t="n">
+        <v>23.96145610278372</v>
+      </c>
+      <c r="E10" t="n">
+        <v>88.77141327623126</v>
+      </c>
+      <c r="F10" t="n">
+        <v>100.4544967880086</v>
+      </c>
+      <c r="G10" t="n">
+        <v>21.63222698072805</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.1730335239697859</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8412769322230743</v>
+      </c>
+      <c r="D11" t="n">
+        <v>32.61223431829963</v>
+      </c>
+      <c r="E11" t="n">
+        <v>88.39450492483152</v>
+      </c>
+      <c r="F11" t="n">
+        <v>110.4271643338517</v>
+      </c>
+      <c r="G11" t="n">
+        <v>17.23224468636599</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1782651100834997</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8283141040512229</v>
+      </c>
+      <c r="D12" t="n">
+        <v>31.91084462982273</v>
+      </c>
+      <c r="E12" t="n">
+        <v>86.67987486965589</v>
+      </c>
+      <c r="F12" t="n">
+        <v>113.633472367049</v>
+      </c>
+      <c r="G12" t="n">
+        <v>21.82012513034411</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>34</v>
+        <v>44</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.169620890396565</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8989907191017944</v>
+      </c>
+      <c r="D13" t="n">
+        <v>29.5310119695321</v>
+      </c>
+      <c r="E13" t="n">
+        <v>90.93362350380849</v>
+      </c>
+      <c r="F13" t="n">
+        <v>109.9646354733406</v>
+      </c>
+      <c r="G13" t="n">
+        <v>21.84058759521219</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.173251042036921</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8441967220738036</v>
+      </c>
+      <c r="D14" t="n">
+        <v>31.04685890834191</v>
+      </c>
+      <c r="E14" t="n">
+        <v>86.90061791967044</v>
+      </c>
+      <c r="F14" t="n">
+        <v>112.711122554068</v>
+      </c>
+      <c r="G14" t="n">
+        <v>20.78836251287333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1663780661615406</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.8809718603253573</v>
+      </c>
+      <c r="D15" t="n">
+        <v>33.56353839245622</v>
+      </c>
+      <c r="E15" t="n">
+        <v>86.79928154467893</v>
+      </c>
+      <c r="F15" t="n">
+        <v>115.3632689717108</v>
+      </c>
+      <c r="G15" t="n">
+        <v>20.40817242927706</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.1658502492317681</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8808121402609804</v>
+      </c>
+      <c r="D16" t="n">
+        <v>27.73424796747967</v>
+      </c>
+      <c r="E16" t="n">
+        <v>88.2428861788618</v>
+      </c>
+      <c r="F16" t="n">
+        <v>107.8272357723577</v>
+      </c>
+      <c r="G16" t="n">
+        <v>13.59146341463415</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>32</v>
+        <v>74</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.1685206107547761</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.8781752109968816</v>
+      </c>
+      <c r="D17" t="n">
+        <v>28.72805507745267</v>
+      </c>
+      <c r="E17" t="n">
+        <v>90.86617900172116</v>
+      </c>
+      <c r="F17" t="n">
+        <v>122.1652323580034</v>
+      </c>
+      <c r="G17" t="n">
+        <v>11.87177280550775</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>37</v>
+        <v>74</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.1834506928529379</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8466548770919182</v>
+      </c>
+      <c r="D18" t="n">
+        <v>31.6819801980198</v>
+      </c>
+      <c r="E18" t="n">
+        <v>86.70653465346534</v>
+      </c>
+      <c r="F18" t="n">
+        <v>120.8641584158416</v>
+      </c>
+      <c r="G18" t="n">
+        <v>11.74178217821782</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>30</v>
+        <v>78</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.1767236012286736</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.878897824486619</v>
+      </c>
+      <c r="D19" t="n">
+        <v>30.18401639344262</v>
+      </c>
+      <c r="E19" t="n">
+        <v>89.72868852459017</v>
+      </c>
+      <c r="F19" t="n">
+        <v>117.5139344262295</v>
+      </c>
+      <c r="G19" t="n">
+        <v>12.0405737704918</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>32</v>
+        <v>70</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.1662980987940527</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.941033328756802</v>
+      </c>
+      <c r="D20" t="n">
+        <v>32.89067974772249</v>
+      </c>
+      <c r="E20" t="n">
+        <v>88.54204625087597</v>
+      </c>
+      <c r="F20" t="n">
+        <v>123.177295024527</v>
+      </c>
+      <c r="G20" t="n">
+        <v>13.89453398738612</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>27</v>
+        <v>71</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.164824341152918</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.8927277137444772</v>
+      </c>
+      <c r="D21" t="n">
+        <v>27.06660666066607</v>
+      </c>
+      <c r="E21" t="n">
+        <v>86.95679567956796</v>
+      </c>
+      <c r="F21" t="n">
+        <v>118.3532853285328</v>
+      </c>
+      <c r="G21" t="n">
+        <v>10.76237623762376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>